<commit_message>
Added Galeria CONTINUA Habana Project
</commit_message>
<xml_diff>
--- a/docs/Pack 1/6. ArteCorte.xlsx
+++ b/docs/Pack 1/6. ArteCorte.xlsx
@@ -731,8 +731,8 @@
   </sheetPr>
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -898,7 +898,7 @@
       <c r="B7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="1" t="s">

</xml_diff>